<commit_message>
funcionando flujo adopcion de recetas y adicion de plantas guadalajara y 7lagoas al server
</commit_message>
<xml_diff>
--- a/flujos_prueba/Vallejo/flujo N Recetas/tables/recetas_VALLEJO.xlsx
+++ b/flujos_prueba/Vallejo/flujo N Recetas/tables/recetas_VALLEJO.xlsx
@@ -132,8 +132,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Recipes_VALLEJO" displayName="Recipes_VALLEJO" ref="A1:L1" headerRowCount="1">
-  <autoFilter ref="A1:L1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Recipes_VALLEJO" displayName="Recipes_VALLEJO" ref="A1:L4" headerRowCount="1">
+  <autoFilter ref="A1:L4"/>
   <tableColumns count="12">
     <tableColumn id="1" name="SKU"/>
     <tableColumn id="2" name="Description"/>
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,6 +525,192 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>300059454</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>DORITOS 3D POPMIX HBSF 120GRX12X1</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Packaging Pellet</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>300059455</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>DORITOS 3D POPMIX HBSF RTD 120GRX12X1</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>Packaging Pellet</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>300059450</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>DORITOS 3D POPMIX HBSF RTDBAU 120GRX12X1</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>Packaging Pellet</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>